<commit_message>
I Have Updated the Status
</commit_message>
<xml_diff>
--- a/Employee_Info/Resource_avilability.xlsx
+++ b/Employee_Info/Resource_avilability.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\JAGADEESH\Palamrutha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\JAGADEESH\Git\WeDoInnovation\Employee_Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>SLNO</t>
   </si>
@@ -446,7 +446,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,7 +483,9 @@
       <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
@@ -497,7 +499,9 @@
       <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
@@ -511,7 +515,9 @@
       <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
@@ -525,7 +531,9 @@
       <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
@@ -539,7 +547,9 @@
       <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>